<commit_message>
Move files into board
</commit_message>
<xml_diff>
--- a/elementalSword/board/Tables.xlsx
+++ b/elementalSword/board/Tables.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samir.farooq\Documents\GitHub\Python-Scripts\elementalSword\board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A369109-4273-4C68-AF0F-EB2A940D9948}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DADA86-B1B4-43E4-9BB6-70633AD8F8C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3276" yWindow="3396" windowWidth="13836" windowHeight="7176" firstSheet="3" activeTab="6" xr2:uid="{DC4BCEDC-BB47-47B4-822F-D357A9FBC158}"/>
-    <workbookView visibility="hidden" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="6" xr2:uid="{BE33DB70-26DA-4DA6-B32B-E004C93227E9}"/>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="8" xr2:uid="{172ED6DA-A762-4758-8CA4-3B66C15DE9E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="6" xr2:uid="{DC4BCEDC-BB47-47B4-822F-D357A9FBC158}"/>
+    <workbookView visibility="hidden" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="6" xr2:uid="{BE33DB70-26DA-4DA6-B32B-E004C93227E9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="8" xr2:uid="{172ED6DA-A762-4758-8CA4-3B66C15DE9E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Encounters" sheetId="8" r:id="rId1"/>
@@ -26,7 +26,6 @@
     <sheet name="Techniques" sheetId="13" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1977,20 +1976,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -2326,17 +2325,17 @@
     <sheetView workbookViewId="1"/>
     <sheetView workbookViewId="2"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="1"/>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>182</v>
       </c>
@@ -2356,7 +2355,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>183</v>
       </c>
@@ -2376,7 +2375,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>81</v>
       </c>
@@ -2396,7 +2395,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="101" t="s">
         <v>194</v>
       </c>
@@ -2416,7 +2415,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="101"/>
       <c r="B5" s="17" t="s">
         <v>196</v>
@@ -2434,7 +2433,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="101"/>
       <c r="B6" t="s">
         <v>198</v>
@@ -2452,7 +2451,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="101"/>
       <c r="B7" s="17" t="s">
         <v>198</v>
@@ -2470,7 +2469,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>206</v>
       </c>
@@ -2490,7 +2489,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>211</v>
       </c>
@@ -2510,7 +2509,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>217</v>
       </c>
@@ -2530,7 +2529,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>218</v>
       </c>
@@ -2550,7 +2549,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>219</v>
       </c>
@@ -2570,7 +2569,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>228</v>
       </c>
@@ -2590,7 +2589,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>234</v>
       </c>
@@ -2610,7 +2609,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>41</v>
       </c>
@@ -2630,7 +2629,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>40</v>
       </c>
@@ -2650,7 +2649,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="60" t="s">
         <v>238</v>
       </c>
@@ -2674,15 +2673,15 @@
     <sheetView workbookViewId="1"/>
     <sheetView workbookViewId="2"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="102" t="s">
         <v>6</v>
@@ -2699,7 +2698,7 @@
       </c>
       <c r="I1" s="104"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -2731,7 +2730,7 @@
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
         <v>3</v>
       </c>
@@ -2760,7 +2759,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -2789,7 +2788,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
         <v>10</v>
       </c>
@@ -2818,7 +2817,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -2847,7 +2846,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
         <v>12</v>
       </c>
@@ -2876,7 +2875,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -2905,7 +2904,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="34" t="s">
         <v>14</v>
       </c>
@@ -2934,7 +2933,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -2963,7 +2962,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
         <v>16</v>
       </c>
@@ -2992,7 +2991,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -3021,7 +3020,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="34" t="s">
         <v>18</v>
       </c>
@@ -3050,7 +3049,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -3079,7 +3078,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="34" t="s">
         <v>20</v>
       </c>
@@ -3108,7 +3107,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
@@ -3137,7 +3136,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>32</v>
       </c>
@@ -3154,7 +3153,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>103</v>
       </c>
@@ -3194,20 +3193,20 @@
     <sheetView workbookViewId="1"/>
     <sheetView workbookViewId="2"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" customWidth="1"/>
-    <col min="6" max="6" width="33.109375" customWidth="1"/>
-    <col min="7" max="7" width="75.5546875" customWidth="1"/>
-    <col min="8" max="8" width="24.5546875" customWidth="1"/>
-    <col min="9" max="9" width="20.109375" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" customWidth="1"/>
+    <col min="6" max="6" width="33.140625" customWidth="1"/>
+    <col min="7" max="7" width="75.5703125" customWidth="1"/>
+    <col min="8" max="8" width="24.5703125" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
@@ -3230,7 +3229,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="105">
         <v>1</v>
       </c>
@@ -3253,7 +3252,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="106"/>
       <c r="B3" s="72">
         <v>2</v>
@@ -3274,7 +3273,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="106"/>
       <c r="B4" s="55">
         <v>3</v>
@@ -3295,7 +3294,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="106"/>
       <c r="B5" s="72">
         <v>4</v>
@@ -3316,7 +3315,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="106"/>
       <c r="B6" s="55">
         <v>5</v>
@@ -3337,7 +3336,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="106"/>
       <c r="B7" s="72">
         <v>6</v>
@@ -3358,7 +3357,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="106"/>
       <c r="B8" s="55">
         <v>7</v>
@@ -3379,7 +3378,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A9" s="107"/>
       <c r="B9" s="76">
         <v>8</v>
@@ -3400,7 +3399,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A10" s="105">
         <v>2</v>
       </c>
@@ -3421,7 +3420,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A11" s="106"/>
       <c r="B11" s="72">
         <v>2</v>
@@ -3440,7 +3439,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A12" s="106"/>
       <c r="B12" s="55">
         <v>3</v>
@@ -3459,7 +3458,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="106"/>
       <c r="B13" s="72">
         <v>4</v>
@@ -3478,7 +3477,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="106"/>
       <c r="B14" s="55">
         <v>5</v>
@@ -3499,7 +3498,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A15" s="106"/>
       <c r="B15" s="72">
         <v>6</v>
@@ -3520,7 +3519,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="106"/>
       <c r="B16" s="55">
         <v>7</v>
@@ -3541,7 +3540,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A17" s="107"/>
       <c r="B17" s="76">
         <v>8</v>
@@ -3562,7 +3561,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A18" s="105">
         <v>3</v>
       </c>
@@ -3585,7 +3584,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="106"/>
       <c r="B19" s="72">
         <v>2</v>
@@ -3606,7 +3605,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A20" s="106"/>
       <c r="B20" s="55">
         <v>3</v>
@@ -3627,7 +3626,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A21" s="106"/>
       <c r="B21" s="72">
         <v>4</v>
@@ -3648,7 +3647,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A22" s="106"/>
       <c r="B22" s="55">
         <v>5</v>
@@ -3669,7 +3668,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A23" s="106"/>
       <c r="B23" s="72">
         <v>6</v>
@@ -3690,7 +3689,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A24" s="106"/>
       <c r="B24" s="55">
         <v>7</v>
@@ -3711,7 +3710,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="107"/>
       <c r="B25" s="76">
         <v>8</v>
@@ -3732,7 +3731,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A26" s="105">
         <v>4</v>
       </c>
@@ -3755,7 +3754,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="27.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="27.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="106"/>
       <c r="B27" s="72">
         <v>2</v>
@@ -3776,7 +3775,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A28" s="106"/>
       <c r="B28" s="55">
         <v>3</v>
@@ -3795,7 +3794,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="23.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="106"/>
       <c r="B29" s="72">
         <v>4</v>
@@ -3816,7 +3815,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="106"/>
       <c r="B30" s="55">
         <v>5</v>
@@ -3837,7 +3836,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A31" s="106"/>
       <c r="B31" s="72">
         <v>6</v>
@@ -3858,7 +3857,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A32" s="106"/>
       <c r="B32" s="55">
         <v>7</v>
@@ -3879,7 +3878,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A33" s="107"/>
       <c r="B33" s="76">
         <v>8</v>
@@ -3900,7 +3899,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="108">
         <v>5</v>
       </c>
@@ -3923,7 +3922,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="108"/>
       <c r="B35" s="79">
         <v>2</v>
@@ -3944,7 +3943,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A36" s="108"/>
       <c r="B36" s="57">
         <v>3</v>
@@ -3965,7 +3964,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A37" s="108"/>
       <c r="B37" s="79">
         <v>4</v>
@@ -3986,7 +3985,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A38" s="108"/>
       <c r="B38" s="57">
         <v>5</v>
@@ -4007,7 +4006,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="24.3" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="24.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="108"/>
       <c r="B39" s="79">
         <v>6</v>
@@ -4028,7 +4027,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="108"/>
       <c r="B40" s="57">
         <v>7</v>
@@ -4049,7 +4048,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A41" s="108"/>
       <c r="B41" s="79">
         <v>8</v>
@@ -4093,14 +4092,14 @@
     <sheetView workbookViewId="1"/>
     <sheetView workbookViewId="2"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.44140625" customWidth="1"/>
-    <col min="3" max="3" width="40.44140625" customWidth="1"/>
-    <col min="4" max="4" width="24.109375" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" customWidth="1"/>
+    <col min="3" max="3" width="40.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>255</v>
       </c>
@@ -4114,7 +4113,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4128,7 +4127,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="62">
         <v>2</v>
       </c>
@@ -4142,7 +4141,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4156,7 +4155,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="62">
         <v>4</v>
       </c>
@@ -4170,7 +4169,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4184,7 +4183,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="62">
         <v>6</v>
       </c>
@@ -4198,7 +4197,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4212,7 +4211,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="62">
         <v>8</v>
       </c>
@@ -4226,7 +4225,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4240,7 +4239,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="62">
         <v>10</v>
       </c>
@@ -4254,7 +4253,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4268,7 +4267,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="62">
         <v>12</v>
       </c>
@@ -4297,15 +4296,15 @@
     <sheetView workbookViewId="1"/>
     <sheetView workbookViewId="2"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="4" max="4" width="38.109375" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="38.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>150</v>
       </c>
@@ -4319,7 +4318,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>318</v>
       </c>
@@ -4333,7 +4332,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="62" t="s">
         <v>319</v>
       </c>
@@ -4347,7 +4346,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>320</v>
       </c>
@@ -4361,7 +4360,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
         <v>321</v>
       </c>
@@ -4375,7 +4374,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>322</v>
       </c>
@@ -4389,7 +4388,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="62" t="s">
         <v>323</v>
       </c>
@@ -4403,7 +4402,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>324</v>
       </c>
@@ -4417,7 +4416,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="62" t="s">
         <v>325</v>
       </c>
@@ -4431,7 +4430,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>326</v>
       </c>
@@ -4445,7 +4444,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="62" t="s">
         <v>327</v>
       </c>
@@ -4459,7 +4458,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>328</v>
       </c>
@@ -4473,7 +4472,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="62" t="s">
         <v>329</v>
       </c>
@@ -4500,15 +4499,15 @@
     <sheetView workbookViewId="1"/>
     <sheetView workbookViewId="2"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" customWidth="1"/>
-    <col min="3" max="18" width="3.6640625" style="11" customWidth="1"/>
-    <col min="19" max="20" width="3.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" customWidth="1"/>
+    <col min="3" max="18" width="3.7109375" style="11" customWidth="1"/>
+    <col min="19" max="20" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="59.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="59.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="7"/>
       <c r="C1" s="14" t="s">
@@ -4566,8 +4565,8 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" s="109" t="s">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="113" t="s">
         <v>60</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -4610,8 +4609,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" s="110"/>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="112"/>
       <c r="B3" s="7" t="s">
         <v>55</v>
       </c>
@@ -4636,7 +4635,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="111" t="s">
         <v>57</v>
       </c>
@@ -4672,8 +4671,8 @@
       <c r="S4" s="18"/>
       <c r="T4" s="30"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A5" s="110"/>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="112"/>
       <c r="B5" s="7" t="s">
         <v>55</v>
       </c>
@@ -4700,7 +4699,7 @@
       <c r="S5" s="19"/>
       <c r="T5" s="31"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="111" t="s">
         <v>58</v>
       </c>
@@ -4738,8 +4737,8 @@
       <c r="S6" s="18"/>
       <c r="T6" s="30"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" s="110"/>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="112"/>
       <c r="B7" s="7" t="s">
         <v>55</v>
       </c>
@@ -4764,7 +4763,7 @@
       <c r="S7" s="19"/>
       <c r="T7" s="31"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="111" t="s">
         <v>59</v>
       </c>
@@ -4800,8 +4799,8 @@
       <c r="S8" s="18"/>
       <c r="T8" s="30"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A9" s="110"/>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="112"/>
       <c r="B9" s="7" t="s">
         <v>55</v>
       </c>
@@ -4828,8 +4827,8 @@
       <c r="S9" s="19"/>
       <c r="T9" s="31"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A10" s="112" t="s">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="109" t="s">
         <v>74</v>
       </c>
       <c r="B10" s="13" t="s">
@@ -4858,8 +4857,8 @@
       <c r="S10" s="18"/>
       <c r="T10" s="30"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A11" s="113"/>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="110"/>
       <c r="B11" s="7" t="s">
         <v>55</v>
       </c>
@@ -4884,8 +4883,8 @@
       <c r="S11" s="19"/>
       <c r="T11" s="31"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" s="112" t="s">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="109" t="s">
         <v>75</v>
       </c>
       <c r="B12" s="13" t="s">
@@ -4920,8 +4919,8 @@
       <c r="S12" s="18"/>
       <c r="T12" s="30"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A13" s="113"/>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="110"/>
       <c r="B13" s="7" t="s">
         <v>55</v>
       </c>
@@ -4946,8 +4945,8 @@
       <c r="S13" s="19"/>
       <c r="T13" s="31"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A14" s="112" t="s">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="109" t="s">
         <v>76</v>
       </c>
       <c r="B14" s="13" t="s">
@@ -4978,8 +4977,8 @@
       <c r="S14" s="18"/>
       <c r="T14" s="30"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A15" s="113"/>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="110"/>
       <c r="B15" s="7" t="s">
         <v>55</v>
       </c>
@@ -5004,8 +5003,8 @@
       <c r="S15" s="19"/>
       <c r="T15" s="31"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A16" s="112" t="s">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="109" t="s">
         <v>77</v>
       </c>
       <c r="B16" s="13" t="s">
@@ -5040,8 +5039,8 @@
       <c r="S16" s="18"/>
       <c r="T16" s="30"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A17" s="113"/>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="110"/>
       <c r="B17" s="7" t="s">
         <v>55</v>
       </c>
@@ -5066,7 +5065,7 @@
       <c r="S17" s="19"/>
       <c r="T17" s="31"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="114" t="s">
         <v>78</v>
       </c>
@@ -5098,8 +5097,8 @@
       <c r="S18" s="22"/>
       <c r="T18" s="30"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A19" s="113"/>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="110"/>
       <c r="B19" s="8" t="s">
         <v>55</v>
       </c>
@@ -5124,7 +5123,7 @@
       <c r="S19" s="22"/>
       <c r="T19" s="31"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="111" t="s">
         <v>71</v>
       </c>
@@ -5156,8 +5155,8 @@
       <c r="S20" s="18"/>
       <c r="T20" s="30"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A21" s="110"/>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="112"/>
       <c r="B21" s="7" t="s">
         <v>55</v>
       </c>
@@ -5182,8 +5181,8 @@
       <c r="S21" s="19"/>
       <c r="T21" s="31"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A22" s="112" t="s">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" s="109" t="s">
         <v>79</v>
       </c>
       <c r="B22" s="13" t="s">
@@ -5218,8 +5217,8 @@
       <c r="S22" s="18"/>
       <c r="T22" s="30"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A23" s="113"/>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="110"/>
       <c r="B23" s="7" t="s">
         <v>55</v>
       </c>
@@ -5244,8 +5243,8 @@
       <c r="S23" s="19"/>
       <c r="T23" s="31"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A24" s="112" t="s">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" s="109" t="s">
         <v>72</v>
       </c>
       <c r="B24" s="13" t="s">
@@ -5276,8 +5275,8 @@
       <c r="S24" s="18"/>
       <c r="T24" s="30"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A25" s="113"/>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" s="110"/>
       <c r="B25" s="7" t="s">
         <v>55</v>
       </c>
@@ -5302,7 +5301,7 @@
       <c r="S25" s="19"/>
       <c r="T25" s="31"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="111" t="s">
         <v>73</v>
       </c>
@@ -5338,8 +5337,8 @@
       <c r="S26" s="18"/>
       <c r="T26" s="30"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A27" s="110"/>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" s="112"/>
       <c r="B27" s="7" t="s">
         <v>55</v>
       </c>
@@ -5364,7 +5363,7 @@
       <c r="S27" s="19"/>
       <c r="T27" s="31"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="111" t="s">
         <v>61</v>
       </c>
@@ -5402,8 +5401,8 @@
       <c r="S28" s="18"/>
       <c r="T28" s="30"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A29" s="110"/>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" s="112"/>
       <c r="B29" s="7" t="s">
         <v>55</v>
       </c>
@@ -5428,7 +5427,7 @@
       <c r="S29" s="19"/>
       <c r="T29" s="31"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="111" t="s">
         <v>62</v>
       </c>
@@ -5460,8 +5459,8 @@
       <c r="S30" s="18"/>
       <c r="T30" s="30"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A31" s="110"/>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" s="112"/>
       <c r="B31" s="7" t="s">
         <v>55</v>
       </c>
@@ -5486,7 +5485,7 @@
       <c r="S31" s="19"/>
       <c r="T31" s="31"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="111" t="s">
         <v>63</v>
       </c>
@@ -5524,8 +5523,8 @@
       <c r="S32" s="18"/>
       <c r="T32" s="30"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A33" s="110"/>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A33" s="112"/>
       <c r="B33" s="7" t="s">
         <v>55</v>
       </c>
@@ -5550,7 +5549,7 @@
       <c r="S33" s="19"/>
       <c r="T33" s="31"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="111" t="s">
         <v>64</v>
       </c>
@@ -5586,8 +5585,8 @@
       <c r="S34" s="18"/>
       <c r="T34" s="30"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A35" s="110"/>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A35" s="112"/>
       <c r="B35" s="7" t="s">
         <v>55</v>
       </c>
@@ -5612,7 +5611,7 @@
       <c r="S35" s="19"/>
       <c r="T35" s="31"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="111" t="s">
         <v>65</v>
       </c>
@@ -5648,8 +5647,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A37" s="110"/>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A37" s="112"/>
       <c r="B37" s="7" t="s">
         <v>55</v>
       </c>
@@ -5674,7 +5673,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="111" t="s">
         <v>54</v>
       </c>
@@ -5712,8 +5711,8 @@
       <c r="S38" s="18"/>
       <c r="T38" s="30"/>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A39" s="110"/>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A39" s="112"/>
       <c r="B39" s="7" t="s">
         <v>55</v>
       </c>
@@ -5738,7 +5737,7 @@
       <c r="S39" s="19"/>
       <c r="T39" s="31"/>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="111" t="s">
         <v>66</v>
       </c>
@@ -5770,8 +5769,8 @@
       <c r="S40" s="18"/>
       <c r="T40" s="30"/>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A41" s="110"/>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A41" s="112"/>
       <c r="B41" s="7" t="s">
         <v>55</v>
       </c>
@@ -5798,7 +5797,7 @@
       <c r="S41" s="19"/>
       <c r="T41" s="31"/>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="111" t="s">
         <v>67</v>
       </c>
@@ -5830,8 +5829,8 @@
       </c>
       <c r="T42" s="30"/>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A43" s="110"/>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A43" s="112"/>
       <c r="B43" s="7" t="s">
         <v>55</v>
       </c>
@@ -5856,7 +5855,7 @@
       </c>
       <c r="T43" s="31"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="111" t="s">
         <v>68</v>
       </c>
@@ -5890,8 +5889,8 @@
       <c r="S44" s="18"/>
       <c r="T44" s="30"/>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A45" s="110"/>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A45" s="112"/>
       <c r="B45" s="7" t="s">
         <v>55</v>
       </c>
@@ -5916,7 +5915,7 @@
       <c r="S45" s="19"/>
       <c r="T45" s="31"/>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="111" t="s">
         <v>53</v>
       </c>
@@ -5952,8 +5951,8 @@
       </c>
       <c r="T46" s="40"/>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A47" s="110"/>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A47" s="112"/>
       <c r="B47" s="7" t="s">
         <v>55</v>
       </c>
@@ -5980,7 +5979,7 @@
       </c>
       <c r="T47" s="31"/>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B48" s="32" t="s">
         <v>82</v>
       </c>
@@ -6057,7 +6056,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>83</v>
       </c>
@@ -6136,6 +6135,16 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A19"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="A46:A47"/>
@@ -6149,16 +6158,6 @@
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A18:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -6173,7 +6172,7 @@
       <selection activeCell="I48" sqref="I48"/>
     </sheetView>
     <sheetView tabSelected="1" workbookViewId="1">
-      <pane xSplit="12552" ySplit="5244" activePane="bottomRight"/>
+      <pane xSplit="12555" ySplit="5250" activePane="bottomRight"/>
       <selection activeCell="U11" sqref="U11"/>
       <selection pane="topRight" activeCell="AC8" sqref="AC8"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
@@ -6181,14 +6180,14 @@
     </sheetView>
     <sheetView workbookViewId="2"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5546875" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" customWidth="1"/>
-    <col min="3" max="27" width="3.6640625" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="27" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="60.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="7"/>
       <c r="C1" s="14" t="s">
@@ -6267,7 +6266,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="115" t="s">
         <v>39</v>
       </c>
@@ -6324,7 +6323,7 @@
       <c r="Z2" s="93"/>
       <c r="AA2" s="91"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="115"/>
       <c r="B3" s="37" t="s">
         <v>105</v>
@@ -6373,7 +6372,7 @@
       <c r="Z3" s="100"/>
       <c r="AA3" s="98"/>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="115"/>
       <c r="B4" s="4" t="s">
         <v>106</v>
@@ -6424,7 +6423,7 @@
       <c r="Z4" s="93"/>
       <c r="AA4" s="91"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="115"/>
       <c r="B5" s="37" t="s">
         <v>107</v>
@@ -6471,7 +6470,7 @@
       <c r="Z5" s="100"/>
       <c r="AA5" s="98"/>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="115"/>
       <c r="B6" s="4" t="s">
         <v>108</v>
@@ -6510,7 +6509,7 @@
       <c r="Z6" s="93"/>
       <c r="AA6" s="91"/>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="115"/>
       <c r="B7" s="37" t="s">
         <v>109</v>
@@ -6549,7 +6548,7 @@
       <c r="Z7" s="100"/>
       <c r="AA7" s="98"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="116"/>
       <c r="B8" s="7" t="s">
         <v>110</v>
@@ -6596,7 +6595,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="117" t="s">
         <v>138</v>
       </c>
@@ -6665,7 +6664,7 @@
       <c r="Z9" s="93"/>
       <c r="AA9" s="91"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="115"/>
       <c r="B10" s="37" t="s">
         <v>112</v>
@@ -6724,7 +6723,7 @@
       <c r="Z10" s="100"/>
       <c r="AA10" s="98"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="115"/>
       <c r="B11" s="4" t="s">
         <v>113</v>
@@ -6775,7 +6774,7 @@
       <c r="Z11" s="93"/>
       <c r="AA11" s="91"/>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="115"/>
       <c r="B12" s="37" t="s">
         <v>114</v>
@@ -6824,7 +6823,7 @@
       <c r="Z12" s="100"/>
       <c r="AA12" s="98"/>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="115"/>
       <c r="B13" s="4" t="s">
         <v>115</v>
@@ -6869,7 +6868,7 @@
       <c r="Z13" s="93"/>
       <c r="AA13" s="91"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="115"/>
       <c r="B14" s="37" t="s">
         <v>116</v>
@@ -6918,7 +6917,7 @@
       <c r="Z14" s="100"/>
       <c r="AA14" s="98"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="115"/>
       <c r="B15" s="4" t="s">
         <v>117</v>
@@ -6961,7 +6960,7 @@
       <c r="Z15" s="93"/>
       <c r="AA15" s="91"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="115"/>
       <c r="B16" s="37" t="s">
         <v>118</v>
@@ -7008,7 +7007,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" s="115"/>
       <c r="B17" s="4" t="s">
         <v>119</v>
@@ -7047,7 +7046,7 @@
       <c r="Z17" s="93"/>
       <c r="AA17" s="91"/>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="115"/>
       <c r="B18" s="37" t="s">
         <v>120</v>
@@ -7088,7 +7087,7 @@
       <c r="Z18" s="100"/>
       <c r="AA18" s="98"/>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="115"/>
       <c r="B19" s="4" t="s">
         <v>121</v>
@@ -7127,7 +7126,7 @@
       <c r="Z19" s="93"/>
       <c r="AA19" s="91"/>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="116"/>
       <c r="B20" s="7" t="s">
         <v>122</v>
@@ -7168,7 +7167,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="117" t="s">
         <v>139</v>
       </c>
@@ -7231,7 +7230,7 @@
       </c>
       <c r="AA21" s="91"/>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="115"/>
       <c r="B22" s="37" t="s">
         <v>124</v>
@@ -7288,7 +7287,7 @@
       </c>
       <c r="AA22" s="98"/>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="115"/>
       <c r="B23" s="4" t="s">
         <v>125</v>
@@ -7345,7 +7344,7 @@
       </c>
       <c r="AA23" s="91"/>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="115"/>
       <c r="B24" s="37" t="s">
         <v>126</v>
@@ -7402,7 +7401,7 @@
       </c>
       <c r="AA24" s="98"/>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="115"/>
       <c r="B25" s="4" t="s">
         <v>127</v>
@@ -7455,7 +7454,7 @@
       </c>
       <c r="AA25" s="91"/>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="115"/>
       <c r="B26" s="37" t="s">
         <v>129</v>
@@ -7504,7 +7503,7 @@
       </c>
       <c r="AA26" s="98"/>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="115"/>
       <c r="B27" s="8" t="s">
         <v>141</v>
@@ -7553,7 +7552,7 @@
       </c>
       <c r="AA27" s="91"/>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" s="115"/>
       <c r="B28" s="37" t="s">
         <v>128</v>
@@ -7602,7 +7601,7 @@
       </c>
       <c r="AA28" s="98"/>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" s="115"/>
       <c r="B29" s="41" t="s">
         <v>131</v>
@@ -7647,7 +7646,7 @@
       </c>
       <c r="AA29" s="91"/>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" s="115"/>
       <c r="B30" s="37" t="s">
         <v>130</v>
@@ -7692,7 +7691,7 @@
       </c>
       <c r="AA30" s="98"/>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" s="115"/>
       <c r="B31" s="41" t="s">
         <v>133</v>
@@ -7737,7 +7736,7 @@
       </c>
       <c r="AA31" s="91"/>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" s="115"/>
       <c r="B32" s="37" t="s">
         <v>132</v>
@@ -7780,7 +7779,7 @@
       </c>
       <c r="AA32" s="98"/>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" s="115"/>
       <c r="B33" s="41" t="s">
         <v>134</v>
@@ -7821,7 +7820,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" s="115"/>
       <c r="B34" s="37" t="s">
         <v>135</v>
@@ -7862,7 +7861,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" s="115"/>
       <c r="B35" s="4" t="s">
         <v>136</v>
@@ -7903,7 +7902,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" s="116"/>
       <c r="B36" s="7" t="s">
         <v>137</v>
@@ -7944,7 +7943,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" s="117" t="s">
         <v>140</v>
       </c>
@@ -7989,7 +7988,7 @@
       <c r="Z37" s="93"/>
       <c r="AA37" s="91"/>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" s="115"/>
       <c r="B38" s="37" t="s">
         <v>62</v>
@@ -8030,7 +8029,7 @@
       <c r="Z38" s="100"/>
       <c r="AA38" s="98"/>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" s="115"/>
       <c r="B39" s="4" t="s">
         <v>63</v>
@@ -8073,7 +8072,7 @@
       <c r="Z39" s="93"/>
       <c r="AA39" s="91"/>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" s="115"/>
       <c r="B40" s="37" t="s">
         <v>64</v>
@@ -8116,7 +8115,7 @@
       <c r="Z40" s="100"/>
       <c r="AA40" s="98"/>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" s="115"/>
       <c r="B41" s="4" t="s">
         <v>65</v>
@@ -8159,7 +8158,7 @@
       <c r="Z41" s="93"/>
       <c r="AA41" s="91"/>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" s="115"/>
       <c r="B42" s="37" t="s">
         <v>54</v>
@@ -8200,7 +8199,7 @@
       <c r="Z42" s="100"/>
       <c r="AA42" s="98"/>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" s="115"/>
       <c r="B43" s="4" t="s">
         <v>66</v>
@@ -8239,7 +8238,7 @@
       <c r="Z43" s="93"/>
       <c r="AA43" s="91"/>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" s="115"/>
       <c r="B44" s="37" t="s">
         <v>67</v>
@@ -8284,7 +8283,7 @@
       <c r="Z44" s="100"/>
       <c r="AA44" s="98"/>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" s="115"/>
       <c r="B45" s="4" t="s">
         <v>68</v>
@@ -8327,7 +8326,7 @@
       <c r="Z45" s="93"/>
       <c r="AA45" s="91"/>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" s="116"/>
       <c r="B46" s="7" t="s">
         <v>53</v>
@@ -8370,7 +8369,7 @@
       <c r="Z46" s="95"/>
       <c r="AA46" s="19"/>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B47" s="32" t="s">
         <v>142</v>
       </c>
@@ -8487,16 +8486,16 @@
     <sheetView workbookViewId="1"/>
     <sheetView workbookViewId="2"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" customWidth="1"/>
-    <col min="4" max="4" width="28.33203125" customWidth="1"/>
-    <col min="5" max="5" width="37.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" customWidth="1"/>
+    <col min="5" max="5" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -8513,7 +8512,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -8530,7 +8529,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
         <v>9</v>
       </c>
@@ -8547,7 +8546,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -8564,7 +8563,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
         <v>11</v>
       </c>
@@ -8581,7 +8580,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -8598,7 +8597,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
         <v>13</v>
       </c>
@@ -8615,7 +8614,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -8632,7 +8631,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="34" t="s">
         <v>15</v>
       </c>
@@ -8649,7 +8648,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -8666,7 +8665,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
         <v>17</v>
       </c>
@@ -8683,7 +8682,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -8700,7 +8699,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="34" t="s">
         <v>19</v>
       </c>
@@ -8717,7 +8716,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -8734,7 +8733,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="34" t="s">
         <v>21</v>
       </c>
@@ -8766,16 +8765,17 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.88671875" customWidth="1"/>
-    <col min="3" max="3" width="100.21875" customWidth="1"/>
-    <col min="4" max="4" width="100.6640625" customWidth="1"/>
-    <col min="5" max="5" width="91.88671875" customWidth="1"/>
-    <col min="6" max="6" width="106.33203125" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="100.28515625" customWidth="1"/>
+    <col min="4" max="4" width="100.7109375" customWidth="1"/>
+    <col min="5" max="5" width="91.85546875" customWidth="1"/>
+    <col min="6" max="6" width="106.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>417</v>
       </c>
@@ -8783,7 +8783,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>434</v>
       </c>
@@ -8800,7 +8800,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -8820,7 +8820,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -8840,7 +8840,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -8860,7 +8860,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -8880,7 +8880,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>435</v>
       </c>
@@ -8900,7 +8900,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -8920,7 +8920,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>435</v>
       </c>
@@ -8940,7 +8940,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="8"/>
       <c r="C10" t="s">
         <v>401</v>
@@ -8955,7 +8955,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -8975,7 +8975,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -8995,7 +8995,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>435</v>
       </c>
@@ -9015,7 +9015,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -9035,7 +9035,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>435</v>
       </c>
@@ -9055,7 +9055,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>44</v>
       </c>
@@ -9075,7 +9075,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" s="8"/>
       <c r="C17" t="s">
         <v>408</v>
@@ -9084,7 +9084,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -9098,7 +9098,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>435</v>
       </c>
@@ -9112,7 +9112,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -9126,7 +9126,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>46</v>
       </c>

</xml_diff>